<commit_message>
public goods working completely
</commit_message>
<xml_diff>
--- a/NGS2 Workflow Logic.xlsx
+++ b/NGS2 Workflow Logic.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="24030"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="17460" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="17460" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="106" uniqueCount="31">
   <si>
     <t>Consent Page</t>
   </si>
@@ -42,9 +42,6 @@
     <t>Initialize</t>
   </si>
   <si>
-    <t>Normal</t>
-  </si>
-  <si>
     <t>Display Only When</t>
   </si>
   <si>
@@ -54,9 +51,6 @@
     <t>SocioDemographic</t>
   </si>
   <si>
-    <t>SET</t>
-  </si>
-  <si>
     <t>demographic</t>
   </si>
   <si>
@@ -91,6 +85,33 @@
   </si>
   <si>
     <t>Only if Ultimatum in app sequence</t>
+  </si>
+  <si>
+    <t>Public Goods Instructions</t>
+  </si>
+  <si>
+    <t>WaitPage</t>
+  </si>
+  <si>
+    <t>OR (p['clicked'] == TRUE) to cover for the cases where we want to force wait till we press start</t>
+  </si>
+  <si>
+    <t>Public Goods</t>
+  </si>
+  <si>
+    <t>Contribute</t>
+  </si>
+  <si>
+    <t>ResultsWaitPage</t>
+  </si>
+  <si>
+    <t>Results</t>
+  </si>
+  <si>
+    <t>NoResponse</t>
+  </si>
+  <si>
+    <t>This page is displayed if a user stopped playing ie didn't contribute anything</t>
   </si>
 </sst>
 </file>
@@ -139,7 +160,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="27">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -167,20 +188,43 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="27">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -194,6 +238,19 @@
     <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -207,6 +264,19 @@
     <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -536,25 +606,25 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="D4:K24"/>
+  <dimension ref="D4:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K25" sqref="K25"/>
+    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="4" max="4" width="12" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="21.83203125" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="26.6640625" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="27.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="4" spans="4:11">
       <c r="D4" s="1" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="G4" t="s">
         <v>1</v>
@@ -569,12 +639,12 @@
         <v>5</v>
       </c>
       <c r="K4" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="5" spans="4:11">
-      <c r="D5" s="3" t="s">
-        <v>12</v>
+      <c r="D5" s="2" t="s">
+        <v>10</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
@@ -593,31 +663,31 @@
       </c>
     </row>
     <row r="6" spans="4:11">
-      <c r="D6" s="3"/>
-      <c r="E6" s="3" t="s">
+      <c r="D6" s="2"/>
+      <c r="E6" s="2" t="s">
         <v>0</v>
       </c>
       <c r="F6" t="s">
+        <v>7</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I6" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J6" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="4:11">
+      <c r="D7" s="2"/>
+      <c r="E7" s="2"/>
+      <c r="F7" t="s">
         <v>8</v>
-      </c>
-      <c r="G6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I6" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J6" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="7" spans="4:11">
-      <c r="D7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="F7" t="s">
-        <v>9</v>
       </c>
       <c r="G7" t="b">
         <v>0</v>
@@ -633,37 +703,37 @@
       </c>
     </row>
     <row r="8" spans="4:11">
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
+      <c r="D8" s="2"/>
+      <c r="E8" s="2" t="s">
+        <v>9</v>
+      </c>
       <c r="F8" t="s">
         <v>7</v>
       </c>
-      <c r="G8" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="H8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="I8" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="J8" s="2" t="s">
+      <c r="G8" t="b">
+        <v>1</v>
+      </c>
+      <c r="H8" t="b">
+        <v>1</v>
+      </c>
+      <c r="I8" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J8" s="1" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="9" spans="4:11">
-      <c r="D9" s="3"/>
-      <c r="E9" s="3" t="s">
-        <v>10</v>
-      </c>
+      <c r="D9" s="2"/>
+      <c r="E9" s="2"/>
       <c r="F9" t="s">
         <v>8</v>
       </c>
-      <c r="G9" t="b">
-        <v>1</v>
+      <c r="G9" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H9" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>3</v>
@@ -673,55 +743,45 @@
       </c>
     </row>
     <row r="10" spans="4:11">
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" t="s">
-        <v>9</v>
-      </c>
-      <c r="G10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H10" t="b">
-        <v>0</v>
-      </c>
-      <c r="I10" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J10" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="D10" s="1"/>
+      <c r="E10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="I10" s="1"/>
+      <c r="J10" s="1"/>
     </row>
     <row r="11" spans="4:11">
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="2" t="s">
+        <v>13</v>
+      </c>
       <c r="F11" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J11" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="12" spans="4:11">
+      <c r="D12" s="2"/>
+      <c r="E12" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F12" t="s">
         <v>7</v>
       </c>
-      <c r="G11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I11" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J11" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="12" spans="4:11">
-      <c r="D12" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F12" t="s">
-        <v>6</v>
-      </c>
-      <c r="G12" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H12" s="1" t="s">
-        <v>3</v>
+      <c r="G12" t="b">
+        <v>1</v>
+      </c>
+      <c r="H12" t="b">
+        <v>1</v>
       </c>
       <c r="I12" s="1" t="s">
         <v>3</v>
@@ -731,18 +791,16 @@
       </c>
     </row>
     <row r="13" spans="4:11">
-      <c r="D13" s="3"/>
-      <c r="E13" s="3" t="s">
-        <v>16</v>
-      </c>
+      <c r="D13" s="2"/>
+      <c r="E13" s="2"/>
       <c r="F13" t="s">
         <v>8</v>
       </c>
-      <c r="G13" t="b">
-        <v>1</v>
-      </c>
-      <c r="H13" t="b">
-        <v>1</v>
+      <c r="G13" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H13" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="I13" s="1" t="s">
         <v>3</v>
@@ -752,72 +810,77 @@
       </c>
     </row>
     <row r="14" spans="4:11">
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="2"/>
+      <c r="E14" s="2" t="s">
+        <v>15</v>
+      </c>
       <c r="F14" t="s">
-        <v>9</v>
-      </c>
-      <c r="G14" s="1" t="s">
-        <v>3</v>
+        <v>7</v>
+      </c>
+      <c r="G14" t="b">
+        <v>1</v>
       </c>
       <c r="H14" t="b">
+        <v>1</v>
+      </c>
+      <c r="I14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J14" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K14" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="4:11">
+      <c r="D15" s="2"/>
+      <c r="E15" s="2"/>
+      <c r="F15" t="s">
+        <v>8</v>
+      </c>
+      <c r="G15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H15" t="b">
         <v>0</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J14" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="15" spans="4:11">
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
-      <c r="F15" t="s">
+      <c r="I15" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J15" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="16" spans="4:11">
+      <c r="D16" s="2"/>
+      <c r="E16" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="F16" t="s">
         <v>7</v>
       </c>
-      <c r="G15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I15" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J15" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="16" spans="4:11">
-      <c r="D16" s="3"/>
-      <c r="E16" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="F16" t="s">
+      <c r="G16" t="b">
+        <v>1</v>
+      </c>
+      <c r="H16" t="b">
+        <v>1</v>
+      </c>
+      <c r="I16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J16" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="K16" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="4:11">
+      <c r="D17" s="2"/>
+      <c r="E17" s="2"/>
+      <c r="F17" t="s">
         <v>8</v>
-      </c>
-      <c r="G16" t="b">
-        <v>1</v>
-      </c>
-      <c r="H16" t="b">
-        <v>1</v>
-      </c>
-      <c r="I16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J16" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="K16" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="17" spans="4:11">
-      <c r="D17" s="3"/>
-      <c r="E17" s="3"/>
-      <c r="F17" t="s">
-        <v>9</v>
       </c>
       <c r="G17" s="1" t="s">
         <v>3</v>
@@ -833,16 +896,18 @@
       </c>
     </row>
     <row r="18" spans="4:11">
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
+      <c r="D18" s="2"/>
+      <c r="E18" s="2" t="s">
+        <v>17</v>
+      </c>
       <c r="F18" t="s">
         <v>7</v>
       </c>
-      <c r="G18" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H18" s="1" t="s">
-        <v>3</v>
+      <c r="G18" t="b">
+        <v>1</v>
+      </c>
+      <c r="H18" t="b">
+        <v>1</v>
       </c>
       <c r="I18" s="1" t="s">
         <v>3</v>
@@ -850,20 +915,21 @@
       <c r="J18" s="1" t="s">
         <v>3</v>
       </c>
+      <c r="K18" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="19" spans="4:11">
-      <c r="D19" s="3"/>
-      <c r="E19" s="3" t="s">
-        <v>18</v>
-      </c>
+      <c r="D19" s="2"/>
+      <c r="E19" s="2"/>
       <c r="F19" t="s">
         <v>8</v>
       </c>
-      <c r="G19" t="b">
-        <v>1</v>
+      <c r="G19" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="H19" t="b">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="I19" s="1" t="s">
         <v>3</v>
@@ -871,61 +937,38 @@
       <c r="J19" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K19" t="s">
+    </row>
+    <row r="21" spans="4:11">
+      <c r="D21" s="2" t="s">
         <v>22</v>
       </c>
-    </row>
-    <row r="20" spans="4:11">
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" t="s">
-        <v>9</v>
-      </c>
-      <c r="G20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H20" t="b">
-        <v>0</v>
-      </c>
-      <c r="I20" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J20" s="1" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="21" spans="4:11">
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="E21" s="2" t="s">
+        <v>23</v>
+      </c>
       <c r="F21" t="s">
         <v>7</v>
       </c>
-      <c r="G21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I21" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J21" s="1" t="s">
-        <v>3</v>
+      <c r="G21" t="b">
+        <v>1</v>
+      </c>
+      <c r="H21" t="b">
+        <v>1</v>
+      </c>
+      <c r="K21" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="22" spans="4:11">
-      <c r="D22" s="3"/>
-      <c r="E22" s="3" t="s">
-        <v>19</v>
-      </c>
+      <c r="D22" s="2"/>
+      <c r="E22" s="2"/>
       <c r="F22" t="s">
         <v>8</v>
       </c>
-      <c r="G22" t="b">
-        <v>1</v>
-      </c>
-      <c r="H22" t="b">
-        <v>1</v>
+      <c r="G22" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="1" t="s">
+        <v>3</v>
       </c>
       <c r="I22" s="1" t="s">
         <v>3</v>
@@ -933,58 +976,317 @@
       <c r="J22" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="K22" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="23" spans="4:11">
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
-      <c r="F23" t="s">
-        <v>9</v>
-      </c>
-      <c r="G23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H23" t="b">
-        <v>0</v>
-      </c>
-      <c r="I23" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J23" s="1" t="s">
-        <v>3</v>
-      </c>
     </row>
     <row r="24" spans="4:11">
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="D24" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="E24" s="2" t="s">
+        <v>26</v>
+      </c>
       <c r="F24" t="s">
         <v>7</v>
       </c>
-      <c r="G24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="H24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="I24" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="J24" s="1" t="s">
-        <v>3</v>
-      </c>
+      <c r="G24" t="b">
+        <v>1</v>
+      </c>
+      <c r="H24" t="b">
+        <v>1</v>
+      </c>
+      <c r="I24" t="b">
+        <v>1</v>
+      </c>
+      <c r="J24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="4:11">
+      <c r="D25" s="2"/>
+      <c r="E25" s="2"/>
+      <c r="F25" t="s">
+        <v>8</v>
+      </c>
+      <c r="G25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H25" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I25" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J25" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="26" spans="4:11">
+      <c r="D26" s="2"/>
+      <c r="E26" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="F26" t="s">
+        <v>7</v>
+      </c>
+      <c r="G26" t="b">
+        <v>1</v>
+      </c>
+      <c r="H26" t="b">
+        <v>1</v>
+      </c>
+      <c r="I26" t="b">
+        <v>1</v>
+      </c>
+      <c r="J26" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="4:11">
+      <c r="D27" s="2"/>
+      <c r="E27" s="2"/>
+      <c r="F27" t="s">
+        <v>8</v>
+      </c>
+      <c r="G27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I27" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J27" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="28" spans="4:11">
+      <c r="D28" s="2"/>
+      <c r="E28" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="F28" t="s">
+        <v>7</v>
+      </c>
+      <c r="G28" t="b">
+        <v>1</v>
+      </c>
+      <c r="H28" t="b">
+        <v>1</v>
+      </c>
+      <c r="I28" t="b">
+        <v>1</v>
+      </c>
+      <c r="J28" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="4:11">
+      <c r="D29" s="2"/>
+      <c r="E29" s="2"/>
+      <c r="F29" t="s">
+        <v>8</v>
+      </c>
+      <c r="G29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I29" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J29" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="30" spans="4:11">
+      <c r="D30" s="2"/>
+      <c r="E30" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="F30" t="s">
+        <v>7</v>
+      </c>
+      <c r="G30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="H30" s="1" t="b">
+        <v>0</v>
+      </c>
+      <c r="I30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="J30" s="1" t="b">
+        <v>1</v>
+      </c>
+      <c r="K30" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="31" spans="4:11">
+      <c r="D31" s="2"/>
+      <c r="E31" s="2"/>
+      <c r="F31" t="s">
+        <v>8</v>
+      </c>
+      <c r="G31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="H31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="I31" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="J31" s="1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="32" spans="4:11">
+      <c r="D32" s="1"/>
+      <c r="E32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+      <c r="I32" s="1"/>
+      <c r="J32" s="1"/>
+    </row>
+    <row r="33" spans="4:10">
+      <c r="D33" s="1"/>
+      <c r="E33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+      <c r="I33" s="1"/>
+      <c r="J33" s="1"/>
+    </row>
+    <row r="34" spans="4:10">
+      <c r="D34" s="1"/>
+      <c r="E34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+      <c r="I34" s="1"/>
+      <c r="J34" s="1"/>
+    </row>
+    <row r="35" spans="4:10">
+      <c r="D35" s="1"/>
+      <c r="E35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+      <c r="I35" s="1"/>
+      <c r="J35" s="1"/>
+    </row>
+    <row r="36" spans="4:10">
+      <c r="D36" s="1"/>
+      <c r="E36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+      <c r="I36" s="1"/>
+      <c r="J36" s="1"/>
+    </row>
+    <row r="37" spans="4:10">
+      <c r="D37" s="1"/>
+      <c r="E37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+      <c r="I37" s="1"/>
+      <c r="J37" s="1"/>
+    </row>
+    <row r="38" spans="4:10">
+      <c r="D38" s="1"/>
+      <c r="E38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+      <c r="I38" s="1"/>
+      <c r="J38" s="1"/>
+    </row>
+    <row r="39" spans="4:10">
+      <c r="D39" s="1"/>
+      <c r="E39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+      <c r="I39" s="1"/>
+      <c r="J39" s="1"/>
+    </row>
+    <row r="40" spans="4:10">
+      <c r="D40" s="1"/>
+      <c r="E40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
+      <c r="I40" s="1"/>
+      <c r="J40" s="1"/>
+    </row>
+    <row r="41" spans="4:10">
+      <c r="D41" s="1"/>
+      <c r="E41" s="1"/>
+      <c r="G41" s="1"/>
+      <c r="H41" s="1"/>
+      <c r="I41" s="1"/>
+      <c r="J41" s="1"/>
+    </row>
+    <row r="42" spans="4:10">
+      <c r="D42" s="1"/>
+      <c r="E42" s="1"/>
+      <c r="G42" s="1"/>
+      <c r="H42" s="1"/>
+      <c r="I42" s="1"/>
+      <c r="J42" s="1"/>
+    </row>
+    <row r="43" spans="4:10">
+      <c r="D43" s="1"/>
+      <c r="E43" s="1"/>
+      <c r="G43" s="1"/>
+      <c r="H43" s="1"/>
+      <c r="I43" s="1"/>
+      <c r="J43" s="1"/>
+    </row>
+    <row r="44" spans="4:10">
+      <c r="D44" s="1"/>
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="4:10">
+      <c r="D45" s="1"/>
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="4:10">
+      <c r="D46" s="1"/>
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="4:10">
+      <c r="D47" s="1"/>
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="4:10">
+      <c r="D48" s="1"/>
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="4:5">
+      <c r="D49" s="1"/>
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="4:5">
+      <c r="D50" s="1"/>
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="4:5">
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="8">
-    <mergeCell ref="E6:E8"/>
-    <mergeCell ref="E9:E11"/>
-    <mergeCell ref="D5:D11"/>
-    <mergeCell ref="D12:D24"/>
-    <mergeCell ref="E13:E15"/>
-    <mergeCell ref="E16:E18"/>
-    <mergeCell ref="E19:E21"/>
-    <mergeCell ref="E22:E24"/>
+  <mergeCells count="15">
+    <mergeCell ref="E21:E22"/>
+    <mergeCell ref="E24:E25"/>
+    <mergeCell ref="E26:E27"/>
+    <mergeCell ref="E28:E29"/>
+    <mergeCell ref="E30:E31"/>
+    <mergeCell ref="D24:D31"/>
+    <mergeCell ref="D21:D22"/>
+    <mergeCell ref="E6:E7"/>
+    <mergeCell ref="E8:E9"/>
+    <mergeCell ref="D5:D9"/>
+    <mergeCell ref="D11:D19"/>
+    <mergeCell ref="E12:E13"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="E16:E17"/>
+    <mergeCell ref="E18:E19"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>